<commit_message>
updated names of project
</commit_message>
<xml_diff>
--- a/Test Plan/Patrick/8_14_to_20_Tests.xlsx
+++ b/Test Plan/Patrick/8_14_to_20_Tests.xlsx
@@ -17,7 +17,7 @@
     <sheet name="Options" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">'PriceCompare Test Plan'!$A$1:$F$23</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">'PriceCompare Test Plan'!$A$1:$G$24</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
@@ -649,14 +649,53 @@
     <xf numFmtId="0" fontId="10" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -666,51 +705,12 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="22">
+  <dxfs count="18">
     <dxf>
       <fill>
         <patternFill>
@@ -750,34 +750,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1123,16 +1095,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:G10" totalsRowShown="0" headerRowDxfId="21" dataDxfId="19" headerRowBorderDxfId="20" tableBorderDxfId="18" totalsRowBorderDxfId="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:G10" totalsRowShown="0" headerRowDxfId="17" dataDxfId="15" headerRowBorderDxfId="16" tableBorderDxfId="14" totalsRowBorderDxfId="13">
   <autoFilter ref="A1:G10"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="Date" dataDxfId="16"/>
-    <tableColumn id="2" name="Sheet" dataDxfId="15"/>
-    <tableColumn id="3" name="Change" dataDxfId="14"/>
-    <tableColumn id="7" name="Modified By" dataDxfId="13"/>
-    <tableColumn id="4" name="Description" dataDxfId="12"/>
-    <tableColumn id="5" name="Comments" dataDxfId="11"/>
-    <tableColumn id="6" name="Version" dataDxfId="10"/>
+    <tableColumn id="1" name="Date" dataDxfId="12"/>
+    <tableColumn id="2" name="Sheet" dataDxfId="11"/>
+    <tableColumn id="3" name="Change" dataDxfId="10"/>
+    <tableColumn id="7" name="Modified By" dataDxfId="9"/>
+    <tableColumn id="4" name="Description" dataDxfId="8"/>
+    <tableColumn id="5" name="Comments" dataDxfId="7"/>
+    <tableColumn id="6" name="Version" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1573,7 +1545,7 @@
   <dimension ref="A1:S24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection sqref="A1:G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1590,70 +1562,70 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="42" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="46" t="s">
+      <c r="A2" s="44" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="47"/>
-      <c r="C2" s="47"/>
-      <c r="D2" s="47"/>
-      <c r="E2" s="47"/>
-      <c r="F2" s="47"/>
+      <c r="B2" s="45"/>
+      <c r="C2" s="45"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="45"/>
+      <c r="F2" s="45"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="52" t="s">
+      <c r="B3" s="50" t="s">
         <v>27</v>
       </c>
-      <c r="C3" s="53"/>
-      <c r="D3" s="53"/>
-      <c r="E3" s="53"/>
-      <c r="F3" s="54"/>
+      <c r="C3" s="51"/>
+      <c r="D3" s="51"/>
+      <c r="E3" s="51"/>
+      <c r="F3" s="52"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="52" t="s">
+      <c r="B4" s="50" t="s">
         <v>28</v>
       </c>
-      <c r="C4" s="53"/>
-      <c r="D4" s="53"/>
-      <c r="E4" s="53"/>
-      <c r="F4" s="54"/>
+      <c r="C4" s="51"/>
+      <c r="D4" s="51"/>
+      <c r="E4" s="51"/>
+      <c r="F4" s="52"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="52" t="s">
+      <c r="B5" s="50" t="s">
         <v>29</v>
       </c>
-      <c r="C5" s="53"/>
-      <c r="D5" s="53"/>
-      <c r="E5" s="53"/>
-      <c r="F5" s="54"/>
+      <c r="C5" s="51"/>
+      <c r="D5" s="51"/>
+      <c r="E5" s="51"/>
+      <c r="F5" s="52"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="51" t="s">
+      <c r="A6" s="49" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="51"/>
-      <c r="C6" s="51"/>
-      <c r="D6" s="51"/>
-      <c r="E6" s="51"/>
-      <c r="F6" s="51"/>
+      <c r="B6" s="49"/>
+      <c r="C6" s="49"/>
+      <c r="D6" s="49"/>
+      <c r="E6" s="49"/>
+      <c r="F6" s="49"/>
       <c r="G6" s="22" t="s">
         <v>6</v>
       </c>
@@ -1662,25 +1634,25 @@
       <c r="A7" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="52"/>
-      <c r="C7" s="53"/>
-      <c r="D7" s="53"/>
-      <c r="E7" s="53"/>
-      <c r="F7" s="54"/>
+      <c r="B7" s="50"/>
+      <c r="C7" s="51"/>
+      <c r="D7" s="51"/>
+      <c r="E7" s="51"/>
+      <c r="F7" s="52"/>
       <c r="G7" s="23">
         <f>COUNTIF(E10:E23,"Y")/ROWS(E10:E23)</f>
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="48" t="s">
+      <c r="A8" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="49"/>
-      <c r="C8" s="49"/>
-      <c r="D8" s="49"/>
-      <c r="E8" s="49"/>
-      <c r="F8" s="50"/>
+      <c r="B8" s="47"/>
+      <c r="C8" s="47"/>
+      <c r="D8" s="47"/>
+      <c r="E8" s="47"/>
+      <c r="F8" s="48"/>
     </row>
     <row r="9" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
@@ -1703,13 +1675,13 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="55" t="s">
+      <c r="A10" s="53" t="s">
         <v>30</v>
       </c>
-      <c r="B10" s="41" t="s">
+      <c r="B10" s="54" t="s">
         <v>31</v>
       </c>
-      <c r="C10" s="38" t="s">
+      <c r="C10" s="39" t="s">
         <v>32</v>
       </c>
       <c r="D10" s="16" t="s">
@@ -1721,9 +1693,9 @@
       <c r="F10" s="24"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="55"/>
-      <c r="B11" s="42"/>
-      <c r="C11" s="39"/>
+      <c r="A11" s="53"/>
+      <c r="B11" s="55"/>
+      <c r="C11" s="41"/>
       <c r="D11" s="16" t="s">
         <v>52</v>
       </c>
@@ -1733,8 +1705,8 @@
       <c r="F11" s="24"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="55"/>
-      <c r="B12" s="43"/>
+      <c r="A12" s="53"/>
+      <c r="B12" s="56"/>
       <c r="C12" s="40"/>
       <c r="D12" s="16" t="s">
         <v>53</v>
@@ -1745,11 +1717,11 @@
       <c r="F12" s="24"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="55"/>
-      <c r="B13" s="41" t="s">
+      <c r="A13" s="53"/>
+      <c r="B13" s="54" t="s">
         <v>34</v>
       </c>
-      <c r="C13" s="38" t="s">
+      <c r="C13" s="39" t="s">
         <v>35</v>
       </c>
       <c r="D13" s="16" t="s">
@@ -1763,8 +1735,8 @@
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="55"/>
-      <c r="B14" s="42"/>
+      <c r="A14" s="53"/>
+      <c r="B14" s="55"/>
       <c r="C14" s="40"/>
       <c r="D14" s="16" t="s">
         <v>37</v>
@@ -1775,9 +1747,9 @@
       <c r="F14" s="24"/>
     </row>
     <row r="15" spans="1:7" ht="24" x14ac:dyDescent="0.25">
-      <c r="A15" s="55"/>
-      <c r="B15" s="42"/>
-      <c r="C15" s="38" t="s">
+      <c r="A15" s="53"/>
+      <c r="B15" s="55"/>
+      <c r="C15" s="39" t="s">
         <v>40</v>
       </c>
       <c r="D15" s="16" t="s">
@@ -1789,9 +1761,9 @@
       <c r="F15" s="24"/>
     </row>
     <row r="16" spans="1:7" ht="24" x14ac:dyDescent="0.25">
-      <c r="A16" s="55"/>
-      <c r="B16" s="42"/>
-      <c r="C16" s="39"/>
+      <c r="A16" s="53"/>
+      <c r="B16" s="55"/>
+      <c r="C16" s="41"/>
       <c r="D16" s="16" t="s">
         <v>41</v>
       </c>
@@ -1801,8 +1773,8 @@
       <c r="F16" s="24"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="55"/>
-      <c r="B17" s="42"/>
+      <c r="A17" s="53"/>
+      <c r="B17" s="55"/>
       <c r="C17" s="40"/>
       <c r="D17" s="16" t="s">
         <v>42</v>
@@ -1813,9 +1785,9 @@
       <c r="F17" s="24"/>
     </row>
     <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="55"/>
-      <c r="B18" s="42"/>
-      <c r="C18" s="38" t="s">
+      <c r="A18" s="53"/>
+      <c r="B18" s="55"/>
+      <c r="C18" s="39" t="s">
         <v>44</v>
       </c>
       <c r="D18" s="16" t="s">
@@ -1827,8 +1799,8 @@
       <c r="F18" s="24"/>
     </row>
     <row r="19" spans="1:6" ht="24" x14ac:dyDescent="0.25">
-      <c r="A19" s="55"/>
-      <c r="B19" s="42"/>
+      <c r="A19" s="53"/>
+      <c r="B19" s="55"/>
       <c r="C19" s="40"/>
       <c r="D19" s="16" t="s">
         <v>45</v>
@@ -1839,8 +1811,8 @@
       <c r="F19" s="24"/>
     </row>
     <row r="20" spans="1:6" ht="24" x14ac:dyDescent="0.25">
-      <c r="A20" s="55"/>
-      <c r="B20" s="42"/>
+      <c r="A20" s="53"/>
+      <c r="B20" s="55"/>
       <c r="C20" s="31" t="s">
         <v>47</v>
       </c>
@@ -1853,8 +1825,8 @@
       <c r="F20" s="24"/>
     </row>
     <row r="21" spans="1:6" ht="24" x14ac:dyDescent="0.25">
-      <c r="A21" s="55"/>
-      <c r="B21" s="42"/>
+      <c r="A21" s="53"/>
+      <c r="B21" s="55"/>
       <c r="C21" s="31" t="s">
         <v>49</v>
       </c>
@@ -1867,9 +1839,9 @@
       <c r="F21" s="24"/>
     </row>
     <row r="22" spans="1:6" ht="24" x14ac:dyDescent="0.25">
-      <c r="A22" s="55"/>
-      <c r="B22" s="42"/>
-      <c r="C22" s="38" t="s">
+      <c r="A22" s="53"/>
+      <c r="B22" s="55"/>
+      <c r="C22" s="39" t="s">
         <v>34</v>
       </c>
       <c r="D22" s="15" t="s">
@@ -1881,8 +1853,8 @@
       <c r="F22" s="24"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="55"/>
-      <c r="B23" s="43"/>
+      <c r="A23" s="53"/>
+      <c r="B23" s="56"/>
       <c r="C23" s="40"/>
       <c r="D23" s="15" t="s">
         <v>51</v>
@@ -1893,7 +1865,7 @@
       <c r="F23" s="26"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D24" s="56"/>
+      <c r="D24" s="38"/>
     </row>
   </sheetData>
   <mergeCells count="16">
@@ -1940,7 +1912,7 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="70" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="50" orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
@@ -1983,6 +1955,28 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <EmailTo xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <EmailHeaders xmlns="http://schemas.microsoft.com/sharepoint/v4" xsi:nil="true"/>
+    <EmailSender xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <EmailFrom xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <EmailSubject xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <EmailCc xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100DACAFF6E33019349B93F2443E7DDCAB9" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8d807c2493d2c3d9870c0a58315e2726">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="http://schemas.microsoft.com/sharepoint/v4" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="86a28fafe5915cae2a78c009e91e23ab" ns1:_="" ns2:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -2151,29 +2145,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{94009DDD-981B-43C7-8CD0-85CDD138DBD0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v4"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <EmailTo xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <EmailHeaders xmlns="http://schemas.microsoft.com/sharepoint/v4" xsi:nil="true"/>
-    <EmailSender xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <EmailFrom xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <EmailSubject xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <EmailCc xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{255CEA57-682A-4711-AA83-3EDFE4A0F805}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07565EDF-20D7-4B2C-8D71-7F1FA2E59011}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2190,29 +2187,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{255CEA57-682A-4711-AA83-3EDFE4A0F805}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{94009DDD-981B-43C7-8CD0-85CDD138DBD0}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v4"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
updated sample code for database evaluator and edited test plan for it
</commit_message>
<xml_diff>
--- a/Test Plan/Patrick/8_14_to_20_Tests.xlsx
+++ b/Test Plan/Patrick/8_14_to_20_Tests.xlsx
@@ -17,7 +17,7 @@
     <sheet name="Options" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">'PriceCompare Test Plan'!$A$1:$G$24</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">'PriceCompare Test Plan'!$A$1:$G$23</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="55">
   <si>
     <t>Application</t>
   </si>
@@ -128,12 +128,6 @@
     <t>N</t>
   </si>
   <si>
-    <t>Client Application Test Plan</t>
-  </si>
-  <si>
-    <t>Test Results for the Client Application</t>
-  </si>
-  <si>
     <t>Patrick Ian E. Cura</t>
   </si>
   <si>
@@ -210,6 +204,15 @@
   </si>
   <si>
     <t>Splahs screen is not resizable</t>
+  </si>
+  <si>
+    <t>Test Plan</t>
+  </si>
+  <si>
+    <t>Test Results for the Database Evaluator Project</t>
+  </si>
+  <si>
+    <t>Database Evaluator</t>
   </si>
 </sst>
 </file>
@@ -298,7 +301,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -365,8 +368,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="15">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -525,15 +534,6 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -649,8 +649,17 @@
     <xf numFmtId="0" fontId="10" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
@@ -694,17 +703,8 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1542,10 +1542,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S24"/>
+  <dimension ref="A1:S34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection sqref="A1:G24"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1562,70 +1562,70 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="42" t="s">
-        <v>26</v>
-      </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
+      <c r="A1" s="45" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="44" t="s">
+      <c r="A2" s="47" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="45"/>
-      <c r="C2" s="45"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="45"/>
-      <c r="F2" s="45"/>
+      <c r="B2" s="48"/>
+      <c r="C2" s="48"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="48"/>
+      <c r="F2" s="48"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="50" t="s">
-        <v>27</v>
-      </c>
-      <c r="C3" s="51"/>
-      <c r="D3" s="51"/>
-      <c r="E3" s="51"/>
-      <c r="F3" s="52"/>
+      <c r="B3" s="53" t="s">
+        <v>53</v>
+      </c>
+      <c r="C3" s="54"/>
+      <c r="D3" s="54"/>
+      <c r="E3" s="54"/>
+      <c r="F3" s="55"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="50" t="s">
-        <v>28</v>
-      </c>
-      <c r="C4" s="51"/>
-      <c r="D4" s="51"/>
-      <c r="E4" s="51"/>
-      <c r="F4" s="52"/>
+      <c r="B4" s="53" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" s="54"/>
+      <c r="D4" s="54"/>
+      <c r="E4" s="54"/>
+      <c r="F4" s="55"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="50" t="s">
-        <v>29</v>
-      </c>
-      <c r="C5" s="51"/>
-      <c r="D5" s="51"/>
-      <c r="E5" s="51"/>
-      <c r="F5" s="52"/>
+      <c r="B5" s="53" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" s="54"/>
+      <c r="D5" s="54"/>
+      <c r="E5" s="54"/>
+      <c r="F5" s="55"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="49" t="s">
+      <c r="A6" s="52" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="49"/>
-      <c r="C6" s="49"/>
-      <c r="D6" s="49"/>
-      <c r="E6" s="49"/>
-      <c r="F6" s="49"/>
+      <c r="B6" s="52"/>
+      <c r="C6" s="52"/>
+      <c r="D6" s="52"/>
+      <c r="E6" s="52"/>
+      <c r="F6" s="52"/>
       <c r="G6" s="22" t="s">
         <v>6</v>
       </c>
@@ -1634,25 +1634,25 @@
       <c r="A7" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="50"/>
-      <c r="C7" s="51"/>
-      <c r="D7" s="51"/>
-      <c r="E7" s="51"/>
-      <c r="F7" s="52"/>
+      <c r="B7" s="53"/>
+      <c r="C7" s="54"/>
+      <c r="D7" s="54"/>
+      <c r="E7" s="54"/>
+      <c r="F7" s="55"/>
       <c r="G7" s="23">
         <f>COUNTIF(E10:E23,"Y")/ROWS(E10:E23)</f>
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="46" t="s">
+      <c r="A8" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="47"/>
-      <c r="C8" s="47"/>
-      <c r="D8" s="47"/>
-      <c r="E8" s="47"/>
-      <c r="F8" s="48"/>
+      <c r="B8" s="50"/>
+      <c r="C8" s="50"/>
+      <c r="D8" s="50"/>
+      <c r="E8" s="50"/>
+      <c r="F8" s="51"/>
     </row>
     <row r="9" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
@@ -1675,200 +1675,347 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="53" t="s">
+      <c r="A10" s="38" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" s="39" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" s="42" t="s">
         <v>30</v>
       </c>
-      <c r="B10" s="54" t="s">
+      <c r="D10" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="C10" s="39" t="s">
+      <c r="E10" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="F10" s="24"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="38"/>
+      <c r="B11" s="40"/>
+      <c r="C11" s="44"/>
+      <c r="D11" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="E11" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="F11" s="24"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="38"/>
+      <c r="B12" s="41"/>
+      <c r="C12" s="43"/>
+      <c r="D12" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="E12" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="F12" s="24"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="38"/>
+      <c r="B13" s="39" t="s">
         <v>32</v>
       </c>
-      <c r="D10" s="16" t="s">
+      <c r="C13" s="42" t="s">
         <v>33</v>
       </c>
-      <c r="E10" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="F10" s="24"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="53"/>
-      <c r="B11" s="55"/>
-      <c r="C11" s="41"/>
-      <c r="D11" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="E11" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="F11" s="24"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="53"/>
-      <c r="B12" s="56"/>
-      <c r="C12" s="40"/>
-      <c r="D12" s="16" t="s">
-        <v>53</v>
-      </c>
-      <c r="E12" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="F12" s="24"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="53"/>
-      <c r="B13" s="54" t="s">
+      <c r="D13" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="E13" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="F13" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="C13" s="39" t="s">
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="38"/>
+      <c r="B14" s="40"/>
+      <c r="C14" s="43"/>
+      <c r="D14" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="D13" s="16" t="s">
+      <c r="E14" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="F14" s="24"/>
+    </row>
+    <row r="15" spans="1:7" ht="24" x14ac:dyDescent="0.25">
+      <c r="A15" s="38"/>
+      <c r="B15" s="40"/>
+      <c r="C15" s="42" t="s">
         <v>38</v>
       </c>
-      <c r="E13" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="F13" s="24" t="s">
+      <c r="D15" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="E15" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="F15" s="24"/>
+    </row>
+    <row r="16" spans="1:7" ht="24" x14ac:dyDescent="0.25">
+      <c r="A16" s="38"/>
+      <c r="B16" s="40"/>
+      <c r="C16" s="44"/>
+      <c r="D16" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="E16" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="F16" s="24"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="38"/>
+      <c r="B17" s="40"/>
+      <c r="C17" s="43"/>
+      <c r="D17" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="E17" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="F17" s="24"/>
+    </row>
+    <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="38"/>
+      <c r="B18" s="40"/>
+      <c r="C18" s="42" t="s">
+        <v>42</v>
+      </c>
+      <c r="D18" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="E18" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="F18" s="24"/>
+    </row>
+    <row r="19" spans="1:6" ht="24" x14ac:dyDescent="0.25">
+      <c r="A19" s="38"/>
+      <c r="B19" s="40"/>
+      <c r="C19" s="43"/>
+      <c r="D19" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="E19" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="F19" s="24"/>
+    </row>
+    <row r="20" spans="1:6" ht="24" x14ac:dyDescent="0.25">
+      <c r="A20" s="38"/>
+      <c r="B20" s="40"/>
+      <c r="C20" s="31" t="s">
+        <v>45</v>
+      </c>
+      <c r="D20" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="E20" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="F20" s="24"/>
+    </row>
+    <row r="21" spans="1:6" ht="24" x14ac:dyDescent="0.25">
+      <c r="A21" s="38"/>
+      <c r="B21" s="40"/>
+      <c r="C21" s="31" t="s">
+        <v>47</v>
+      </c>
+      <c r="D21" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="E21" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="F21" s="24"/>
+    </row>
+    <row r="22" spans="1:6" ht="24" x14ac:dyDescent="0.25">
+      <c r="A22" s="38"/>
+      <c r="B22" s="40"/>
+      <c r="C22" s="42" t="s">
+        <v>32</v>
+      </c>
+      <c r="D22" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="E22" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="F22" s="24"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="38"/>
+      <c r="B23" s="41"/>
+      <c r="C23" s="43"/>
+      <c r="D23" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="E23" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="F23" s="26"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="56" t="s">
+        <v>54</v>
+      </c>
+      <c r="B24" s="39" t="s">
+        <v>32</v>
+      </c>
+      <c r="C24" s="42" t="s">
+        <v>33</v>
+      </c>
+      <c r="D24" s="16" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="53"/>
-      <c r="B14" s="55"/>
-      <c r="C14" s="40"/>
-      <c r="D14" s="16" t="s">
+      <c r="E24" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="F24" s="24" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="56"/>
+      <c r="B25" s="40"/>
+      <c r="C25" s="43"/>
+      <c r="D25" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="E25" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="F25" s="24"/>
+    </row>
+    <row r="26" spans="1:6" ht="24" x14ac:dyDescent="0.25">
+      <c r="A26" s="56"/>
+      <c r="B26" s="40"/>
+      <c r="C26" s="42" t="s">
+        <v>38</v>
+      </c>
+      <c r="D26" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="E14" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="F14" s="24"/>
-    </row>
-    <row r="15" spans="1:7" ht="24" x14ac:dyDescent="0.25">
-      <c r="A15" s="53"/>
-      <c r="B15" s="55"/>
-      <c r="C15" s="39" t="s">
+      <c r="E26" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="F26" s="24"/>
+    </row>
+    <row r="27" spans="1:6" ht="24" x14ac:dyDescent="0.25">
+      <c r="A27" s="56"/>
+      <c r="B27" s="40"/>
+      <c r="C27" s="44"/>
+      <c r="D27" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="E27" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="F27" s="24"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="56"/>
+      <c r="B28" s="40"/>
+      <c r="C28" s="43"/>
+      <c r="D28" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="D15" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="E15" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="F15" s="24"/>
-    </row>
-    <row r="16" spans="1:7" ht="24" x14ac:dyDescent="0.25">
-      <c r="A16" s="53"/>
-      <c r="B16" s="55"/>
-      <c r="C16" s="41"/>
-      <c r="D16" s="16" t="s">
+      <c r="E28" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="F28" s="24"/>
+    </row>
+    <row r="29" spans="1:6" ht="24" x14ac:dyDescent="0.25">
+      <c r="A29" s="56"/>
+      <c r="B29" s="40"/>
+      <c r="C29" s="42" t="s">
+        <v>42</v>
+      </c>
+      <c r="D29" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="E16" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="F16" s="24"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="53"/>
-      <c r="B17" s="55"/>
-      <c r="C17" s="40"/>
-      <c r="D17" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="E17" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="F17" s="24"/>
-    </row>
-    <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="53"/>
-      <c r="B18" s="55"/>
-      <c r="C18" s="39" t="s">
+      <c r="E29" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="F29" s="24"/>
+    </row>
+    <row r="30" spans="1:6" ht="24" x14ac:dyDescent="0.25">
+      <c r="A30" s="56"/>
+      <c r="B30" s="40"/>
+      <c r="C30" s="43"/>
+      <c r="D30" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="E30" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="F30" s="24"/>
+    </row>
+    <row r="31" spans="1:6" ht="24" x14ac:dyDescent="0.25">
+      <c r="A31" s="56"/>
+      <c r="B31" s="40"/>
+      <c r="C31" s="31" t="s">
+        <v>45</v>
+      </c>
+      <c r="D31" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="D18" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="E18" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="F18" s="24"/>
-    </row>
-    <row r="19" spans="1:6" ht="24" x14ac:dyDescent="0.25">
-      <c r="A19" s="53"/>
-      <c r="B19" s="55"/>
-      <c r="C19" s="40"/>
-      <c r="D19" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="E19" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="F19" s="24"/>
-    </row>
-    <row r="20" spans="1:6" ht="24" x14ac:dyDescent="0.25">
-      <c r="A20" s="53"/>
-      <c r="B20" s="55"/>
-      <c r="C20" s="31" t="s">
+      <c r="E31" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="F31" s="24"/>
+    </row>
+    <row r="32" spans="1:6" ht="24" x14ac:dyDescent="0.25">
+      <c r="A32" s="56"/>
+      <c r="B32" s="40"/>
+      <c r="C32" s="31" t="s">
         <v>47</v>
       </c>
-      <c r="D20" s="16" t="s">
+      <c r="D32" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="E20" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="F20" s="24"/>
-    </row>
-    <row r="21" spans="1:6" ht="24" x14ac:dyDescent="0.25">
-      <c r="A21" s="53"/>
-      <c r="B21" s="55"/>
-      <c r="C21" s="31" t="s">
+      <c r="E32" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="F32" s="24"/>
+    </row>
+    <row r="33" spans="1:6" ht="24" x14ac:dyDescent="0.25">
+      <c r="A33" s="56"/>
+      <c r="B33" s="40"/>
+      <c r="C33" s="42" t="s">
+        <v>32</v>
+      </c>
+      <c r="D33" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="E33" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="F33" s="24"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="56"/>
+      <c r="B34" s="41"/>
+      <c r="C34" s="43"/>
+      <c r="D34" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="D21" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="E21" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="F21" s="24"/>
-    </row>
-    <row r="22" spans="1:6" ht="24" x14ac:dyDescent="0.25">
-      <c r="A22" s="53"/>
-      <c r="B22" s="55"/>
-      <c r="C22" s="39" t="s">
-        <v>34</v>
-      </c>
-      <c r="D22" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="E22" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="F22" s="24"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="53"/>
-      <c r="B23" s="56"/>
-      <c r="C23" s="40"/>
-      <c r="D23" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="E23" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="F23" s="26"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D24" s="38"/>
+      <c r="E34" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="F34" s="26"/>
     </row>
   </sheetData>
-  <mergeCells count="16">
+  <mergeCells count="22">
     <mergeCell ref="C22:C23"/>
     <mergeCell ref="C18:C19"/>
     <mergeCell ref="C15:C17"/>
@@ -1885,29 +2032,35 @@
     <mergeCell ref="B10:B12"/>
     <mergeCell ref="C10:C12"/>
     <mergeCell ref="B13:B23"/>
+    <mergeCell ref="A24:A34"/>
+    <mergeCell ref="B24:B34"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="C26:C28"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="C33:C34"/>
   </mergeCells>
   <conditionalFormatting sqref="G7">
-    <cfRule type="cellIs" dxfId="5" priority="27" operator="lessThan">
+    <cfRule type="cellIs" dxfId="5" priority="29" operator="lessThan">
       <formula>0.5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="28" operator="lessThan">
+    <cfRule type="cellIs" dxfId="4" priority="30" operator="lessThan">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="31" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="30" operator="equal">
+    <cfRule type="cellIs" priority="32" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="33" operator="equal">
       <formula>100</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E10:E23">
-    <cfRule type="cellIs" dxfId="1" priority="25" operator="equal">
+  <conditionalFormatting sqref="E10:E34">
+    <cfRule type="cellIs" dxfId="1" priority="27" operator="equal">
       <formula>"N"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="28" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1921,7 +2074,7 @@
           <x14:formula1>
             <xm:f>Options!$A$1:$A$2</xm:f>
           </x14:formula1>
-          <xm:sqref>E10:E23</xm:sqref>
+          <xm:sqref>E10:E34</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>